<commit_message>
First implementation of algorithm.
</commit_message>
<xml_diff>
--- a/bushnaq-family.xlsx
+++ b/bushnaq-family.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -88,10 +88,7 @@
     <t xml:space="preserve">Josting</t>
   </si>
   <si>
-    <t xml:space="preserve">Constanze Shuruq Shuruq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bushnaq Josting</t>
+    <t xml:space="preserve">Constanze Shuruq Magnolia</t>
   </si>
 </sst>
 </file>
@@ -196,10 +193,10 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -315,7 +312,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>23857</v>
+        <v>24222</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="0" t="str">
@@ -388,7 +385,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>34398</v>
+        <v>35129</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="0" t="str">
@@ -431,10 +428,10 @@
         <v>22</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>36025</v>
+        <v>36756</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="0" t="str">

</xml_diff>